<commit_message>
Aenderungen an Konjunkturverlauf, Angebot und Nachfrage waehrend Praesentation
</commit_message>
<xml_diff>
--- a/20 Spielwelt/20 Storyline/20110926 Konjunturverlauf.xlsx
+++ b/20 Spielwelt/20 Storyline/20110926 Konjunturverlauf.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="27315" windowHeight="13350"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="15600" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="Diagramm1" sheetId="4" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId2"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId3"/>
+    <sheet name="Tabelle3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -208,7 +209,85 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="41618944"/>
+        <c:axId val="62599104"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="41618944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="62599104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="62599104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="41618944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -796,11 +875,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101778176"/>
-        <c:axId val="101780864"/>
+        <c:axId val="41616896"/>
+        <c:axId val="62617216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101778176"/>
+        <c:axId val="41616896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -809,7 +888,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101780864"/>
+        <c:crossAx val="62617216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -817,7 +896,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101780864"/>
+        <c:axId val="62617216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -828,7 +907,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101778176"/>
+        <c:crossAx val="41616896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -850,7 +929,45 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="88" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9308523" cy="6018068"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1174,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Konkunkturverlauf auch fuer Personalkosten und anhand von Datenbasis
</commit_message>
<xml_diff>
--- a/20 Spielwelt/20 Storyline/20110926 Konjunturverlauf.xlsx
+++ b/20 Spielwelt/20 Storyline/20110926 Konjunturverlauf.xlsx
@@ -4,20 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="15600" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="9600" windowHeight="12600"/>
   </bookViews>
   <sheets>
-    <sheet name="Diagramm1" sheetId="4" r:id="rId1"/>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId2"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId3"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId4"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Nachfrage</t>
   </si>
@@ -77,6 +76,9 @@
   </si>
   <si>
     <t>ohne Warp</t>
+  </si>
+  <si>
+    <t>Personalkosten</t>
   </si>
 </sst>
 </file>
@@ -174,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -192,6 +194,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -209,85 +214,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="41618944"/>
-        <c:axId val="62599104"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="41618944"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62599104"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="62599104"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41618944"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -366,34 +293,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -462,34 +389,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -558,34 +485,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -663,21 +590,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -754,21 +666,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -845,21 +742,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -875,11 +757,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="41616896"/>
-        <c:axId val="62617216"/>
+        <c:axId val="104363136"/>
+        <c:axId val="104364672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="41616896"/>
+        <c:axId val="104363136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -888,7 +770,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62617216"/>
+        <c:crossAx val="104364672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -896,7 +778,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62617216"/>
+        <c:axId val="104364672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -907,7 +789,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41616896"/>
+        <c:crossAx val="104363136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -929,58 +811,20 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr/>
-  <sheetViews>
-    <sheetView zoomScale="88" workbookViewId="0" zoomToFit="1"/>
-  </sheetViews>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</chartsheet>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9308523" cy="6018068"/>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Diagramm 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks noGrp="1"/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:absoluteAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>885824</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>857249</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1289,15 +1133,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
@@ -1366,34 +1210,34 @@
         <v>2</v>
       </c>
       <c r="B5" s="8">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="C5" s="8">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="D5" s="8">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="E5" s="8">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="F5" s="8">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="G5" s="8">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="H5" s="8">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="I5" s="8">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="J5" s="8">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="K5" s="8">
-        <v>13</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1401,34 +1245,34 @@
         <v>3</v>
       </c>
       <c r="B6" s="8">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="C6" s="8">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="D6" s="8">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="E6" s="8">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="F6" s="8">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="G6" s="8">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="H6" s="8">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="I6" s="8">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="J6" s="8">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="K6" s="8">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1436,55 +1280,45 @@
         <v>4</v>
       </c>
       <c r="B7" s="8">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C7" s="8">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D7" s="8">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="E7" s="8">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="F7" s="8">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="G7" s="8">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="H7" s="8">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="I7" s="8">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="J7" s="8">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="K7" s="8">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="8">
-        <v>9</v>
-      </c>
-      <c r="F8" s="8">
-        <v>5</v>
-      </c>
-      <c r="G8" s="8">
-        <v>2</v>
-      </c>
-      <c r="H8" s="8">
-        <v>1</v>
-      </c>
-      <c r="I8" s="8">
-        <v>0</v>
-      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
     </row>
@@ -1492,21 +1326,11 @@
       <c r="A9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="8">
-        <v>7</v>
-      </c>
-      <c r="F9" s="8">
-        <v>4</v>
-      </c>
-      <c r="G9" s="8">
-        <v>2</v>
-      </c>
-      <c r="H9" s="8">
-        <v>1</v>
-      </c>
-      <c r="I9" s="8">
-        <v>0</v>
-      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
     </row>
@@ -1514,23 +1338,48 @@
       <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="8">
-        <v>10</v>
-      </c>
-      <c r="F10" s="8">
-        <v>6</v>
-      </c>
-      <c r="G10" s="8">
-        <v>3</v>
-      </c>
-      <c r="H10" s="8">
-        <v>1</v>
-      </c>
-      <c r="I10" s="8">
-        <v>0</v>
-      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
+    </row>
+    <row r="11" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="8">
+        <v>10</v>
+      </c>
+      <c r="C11" s="8">
+        <v>10</v>
+      </c>
+      <c r="D11" s="8">
+        <v>15</v>
+      </c>
+      <c r="E11" s="8">
+        <v>12</v>
+      </c>
+      <c r="F11" s="8">
+        <v>10</v>
+      </c>
+      <c r="G11" s="8">
+        <v>10</v>
+      </c>
+      <c r="H11" s="8">
+        <v>8</v>
+      </c>
+      <c r="I11" s="8">
+        <v>9</v>
+      </c>
+      <c r="J11" s="8">
+        <v>12</v>
+      </c>
+      <c r="K11" s="8">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>